<commit_message>
Alterações Finais na página Fale Conosco
</commit_message>
<xml_diff>
--- a/Documentação/Backlog/Backlog - Grupo 04.xlsx
+++ b/Documentação/Backlog/Backlog - Grupo 04.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Desktop\Git\Meus-repositorios\Projeto_PI\sprint2\Backlog\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Desktop\Git\Meus-repositorios\Projeto_PI\sprint2\Documentação\Backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02E06AC7-92BA-4B49-A933-764A93914A04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{385BD36F-1989-486D-AFE8-F4F060C63755}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2480,19 +2480,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6A7E6C11-E15E-43D4-8193-0A9DA9700B3C}" name="Tabela2" displayName="Tabela2" ref="A2:J51" totalsRowShown="0" headerRowDxfId="24" tableBorderDxfId="23">
-  <autoFilter ref="A2:J51" xr:uid="{6A7E6C11-E15E-43D4-8193-0A9DA9700B3C}">
-    <filterColumn colId="6">
-      <filters>
-        <filter val="2"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="7">
-      <filters>
-        <filter val="Em Andamento"/>
-        <filter val="Pendente"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A2:J51" xr:uid="{6A7E6C11-E15E-43D4-8193-0A9DA9700B3C}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:J43">
     <sortCondition ref="G3:G43"/>
     <sortCondition ref="C3:C43"/>
@@ -2793,8 +2781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M51"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -2858,7 +2846,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="31" hidden="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -2891,7 +2879,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="46.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
@@ -2924,7 +2912,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="46.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
@@ -2957,7 +2945,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="62" hidden="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" ht="62" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
@@ -2990,7 +2978,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="46.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
@@ -3024,7 +3012,7 @@
       </c>
       <c r="L7" s="5"/>
     </row>
-    <row r="8" spans="1:13" ht="31" hidden="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
@@ -3057,7 +3045,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="46.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>0</v>
       </c>
@@ -3091,7 +3079,7 @@
       </c>
       <c r="M9"/>
     </row>
-    <row r="10" spans="1:13" ht="31" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>13</v>
       </c>
@@ -3124,7 +3112,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="46.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>8</v>
       </c>
@@ -3157,7 +3145,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="31" hidden="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>4</v>
       </c>
@@ -3190,7 +3178,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="31" hidden="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>11</v>
       </c>
@@ -3223,7 +3211,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="31" hidden="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>12</v>
       </c>
@@ -3280,7 +3268,7 @@
         <v>2</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I15" s="2" t="s">
         <v>103</v>
@@ -3388,7 +3376,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="46.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
         <v>56</v>
       </c>
@@ -3421,7 +3409,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="31" hidden="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" ht="31" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
         <v>26</v>
       </c>
@@ -3454,7 +3442,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="46.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
         <v>27</v>
       </c>
@@ -3487,7 +3475,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
         <v>18</v>
       </c>
@@ -3553,7 +3541,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="31" hidden="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" ht="31" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
         <v>42</v>
       </c>
@@ -3586,7 +3574,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="31" hidden="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" ht="31" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
         <v>25</v>
       </c>
@@ -3619,7 +3607,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="31" hidden="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" ht="31" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
         <v>57</v>
       </c>
@@ -3652,7 +3640,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="s">
         <v>28</v>
       </c>
@@ -3685,7 +3673,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="31" hidden="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" ht="31" x14ac:dyDescent="0.35">
       <c r="A28" s="4" t="s">
         <v>29</v>
       </c>
@@ -3775,7 +3763,7 @@
         <v>2</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I30" s="2" t="s">
         <v>106</v>
@@ -3784,7 +3772,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
         <v>20</v>
       </c>
@@ -3841,7 +3829,7 @@
         <v>2</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I32" s="2" t="s">
         <v>104</v>
@@ -3883,7 +3871,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" s="4" t="s">
         <v>47</v>
       </c>
@@ -3916,7 +3904,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
         <v>46</v>
       </c>
@@ -3949,7 +3937,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36" s="4" t="s">
         <v>45</v>
       </c>
@@ -3982,7 +3970,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37" s="4" t="s">
         <v>43</v>
       </c>
@@ -4015,7 +4003,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38" s="4" t="s">
         <v>48</v>
       </c>
@@ -4048,7 +4036,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39" s="4" t="s">
         <v>49</v>
       </c>
@@ -4081,7 +4069,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40" s="4" t="s">
         <v>50</v>
       </c>
@@ -4114,7 +4102,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41" s="4" t="s">
         <v>51</v>
       </c>
@@ -4147,7 +4135,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="42" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42" s="4" t="s">
         <v>44</v>
       </c>
@@ -4180,7 +4168,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="31" hidden="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" ht="31" x14ac:dyDescent="0.35">
       <c r="A43" s="4" t="s">
         <v>62</v>
       </c>
@@ -4213,7 +4201,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44" s="4" t="s">
         <v>94</v>
       </c>
@@ -4246,7 +4234,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A45" s="4" t="s">
         <v>95</v>
       </c>
@@ -4279,7 +4267,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46" s="4" t="s">
         <v>19</v>
       </c>
@@ -4312,7 +4300,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="47" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47" s="4" t="s">
         <v>96</v>
       </c>
@@ -4345,7 +4333,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="48" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A48" s="4" t="s">
         <v>97</v>
       </c>
@@ -4378,7 +4366,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="49" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A49" s="4" t="s">
         <v>98</v>
       </c>
@@ -4411,7 +4399,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="50" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A50" s="4" t="s">
         <v>99</v>
       </c>
@@ -4444,7 +4432,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="51" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A51" s="4" t="s">
         <v>100</v>
       </c>

</xml_diff>

<commit_message>
Ajustes para a apresentação
</commit_message>
<xml_diff>
--- a/Documentação/Backlog/Backlog - Grupo 04.xlsx
+++ b/Documentação/Backlog/Backlog - Grupo 04.xlsx
@@ -5,16 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Desktop\Git\Meus-repositorios\Projeto_PI\sprint2\Documentação\Backlog\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpfer\OneDrive\Documentos\SPTECH\PI\SPRINT\Sprint-SPTECH\Documentação\Backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{385BD36F-1989-486D-AFE8-F4F060C63755}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE2EAAA9-2B34-42D8-805E-B46A6C434DB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
     <sheet name="Burndow" sheetId="2" r:id="rId2"/>
+    <sheet name="Burndow - Sprint2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="118">
   <si>
     <t>Configuração e instalação do Arduino Uno R3 com Sensor MQ-2 utilizando Protoboard e 3 Jumpers (Macho-Macho).</t>
   </si>
@@ -401,6 +402,18 @@
   </si>
   <si>
     <t>TOTAL</t>
+  </si>
+  <si>
+    <t>2A</t>
+  </si>
+  <si>
+    <t>2B</t>
+  </si>
+  <si>
+    <t>2C</t>
+  </si>
+  <si>
+    <t>2D</t>
   </si>
 </sst>
 </file>
@@ -645,7 +658,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
+  <dxfs count="32">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -705,6 +718,122 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="medium">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="medium">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="medium">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFCB0000"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1881,6 +2010,863 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1260" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR" b="1"/>
+              <a:t>BURNDOW</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="3.5833333333333117E-3"/>
+          <c:y val="1.3888888888888888E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1260" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="7.0914260717410318E-2"/>
+          <c:y val="0.24520888013998252"/>
+          <c:w val="0.89019685039370078"/>
+          <c:h val="0.67053988043161272"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Burndow - Sprint2'!$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>TOTAL</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Burndow - Sprint2'!$B$3:$B$8</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>('Burndow - Sprint2'!$B$3,'Burndow - Sprint2'!$B$5:$B$8)</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>TOTAL</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2A</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2B</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2C</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2D</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Burndow - Sprint2'!$B$3:$B$8</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>('Burndow - Sprint2'!$B$3,'Burndow - Sprint2'!$B$5:$B$8)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-22E1-4CBE-B438-D71EBB8520F0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Burndow - Sprint2'!$C$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Pontos Planejados</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.8166666666666691E-2"/>
+                  <c:y val="-5.7835739282589678E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-22E1-4CBE-B438-D71EBB8520F0}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.2611111111111113E-2"/>
+                  <c:y val="3.01272236803732E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-22E1-4CBE-B438-D71EBB8520F0}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.0944444444444445E-2"/>
+                  <c:y val="2.5497594050743571E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-22E1-4CBE-B438-D71EBB8520F0}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.7500235563576936E-2"/>
+                  <c:y val="-9.5375773277822738E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000B-22E1-4CBE-B438-D71EBB8520F0}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Burndow - Sprint2'!$B$3:$B$8</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>('Burndow - Sprint2'!$B$3,'Burndow - Sprint2'!$B$5:$B$8)</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>TOTAL</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2A</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2B</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2C</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2D</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Burndow - Sprint2'!$C$3:$C$8</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>('Burndow - Sprint2'!$C$3,'Burndow - Sprint2'!$C$5:$C$8)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>29</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-22E1-4CBE-B438-D71EBB8520F0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Burndow - Sprint2'!$D$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Pontos Realizados</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.0944444444444445E-2"/>
+                  <c:y val="3.9386482939632504E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-22E1-4CBE-B438-D71EBB8520F0}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.3500000000000002E-2"/>
+                  <c:y val="3.4756853310002833E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000006-22E1-4CBE-B438-D71EBB8520F0}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.5388888888888888E-2"/>
+                  <c:y val="-3.0057961504811985E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000007-22E1-4CBE-B438-D71EBB8520F0}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.2611111111111113E-2"/>
+                  <c:y val="-3.4687591134441531E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000008-22E1-4CBE-B438-D71EBB8520F0}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.7500235563576936E-2"/>
+                  <c:y val="-6.9196883870551534E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000A-22E1-4CBE-B438-D71EBB8520F0}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Burndow - Sprint2'!$B$3:$B$8</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>('Burndow - Sprint2'!$B$3,'Burndow - Sprint2'!$B$5:$B$8)</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>TOTAL</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2A</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2B</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2C</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2D</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Burndow - Sprint2'!$D$3:$D$8</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>('Burndow - Sprint2'!$D$3,'Burndow - Sprint2'!$D$5:$D$8)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>35</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-22E1-4CBE-B438-D71EBB8520F0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="t"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1937044160"/>
+        <c:axId val="1937044640"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1937044160"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1937044640"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1937044640"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1937044160"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.67850743657042856"/>
+          <c:y val="2.3726305045202681E-2"/>
+          <c:w val="0.32076268591426071"/>
+          <c:h val="0.25868110236220471"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:srgbClr val="CB0000"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1050">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1921,7 +2907,563 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2478,8 +4020,51 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>250824</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1586</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>251460</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>7619</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A26A1CD-D56A-404D-AF02-F3009ABDC1FC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6A7E6C11-E15E-43D4-8193-0A9DA9700B3C}" name="Tabela2" displayName="Tabela2" ref="A2:J51" totalsRowShown="0" headerRowDxfId="24" tableBorderDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6A7E6C11-E15E-43D4-8193-0A9DA9700B3C}" name="Tabela2" displayName="Tabela2" ref="A2:J51" totalsRowShown="0" headerRowDxfId="31" tableBorderDxfId="30">
   <autoFilter ref="A2:J51" xr:uid="{6A7E6C11-E15E-43D4-8193-0A9DA9700B3C}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:J43">
     <sortCondition ref="G3:G43"/>
@@ -2487,30 +4072,44 @@
     <sortCondition ref="F3:F43"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{9F7D184E-A2F2-4E3C-AF8D-4C0F7A1EB03C}" name="Requisito" dataDxfId="22"/>
-    <tableColumn id="9" xr3:uid="{B9B864BA-C5E5-45E2-817E-3E3871CAC849}" name="Descrição" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{7736CB43-35DE-44E3-99F9-A059BE9A77F6}" name="Classificação" dataDxfId="20"/>
-    <tableColumn id="7" xr3:uid="{3502BB37-E611-4076-B136-7B67D26992FF}" name="Tamanho " dataDxfId="19">
+    <tableColumn id="1" xr3:uid="{9F7D184E-A2F2-4E3C-AF8D-4C0F7A1EB03C}" name="Requisito" dataDxfId="29"/>
+    <tableColumn id="9" xr3:uid="{B9B864BA-C5E5-45E2-817E-3E3871CAC849}" name="Descrição" dataDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{7736CB43-35DE-44E3-99F9-A059BE9A77F6}" name="Classificação" dataDxfId="27"/>
+    <tableColumn id="7" xr3:uid="{3502BB37-E611-4076-B136-7B67D26992FF}" name="Tamanho " dataDxfId="26">
       <calculatedColumnFormula array="1">_xlfn.IFS(E3=3,"PP",E3=5,"P",E3=8,"M",E3=13,"G",E3=21,"GG")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{04F91C54-26E1-4063-B34C-03486B3A493F}" name="Tamanho (#)" dataDxfId="18"/>
-    <tableColumn id="8" xr3:uid="{203EEE87-31C9-4EC2-8FF5-1485A10738C6}" name="Prioridade" dataDxfId="17"/>
-    <tableColumn id="10" xr3:uid="{BD2690E1-9135-40F1-9CE5-CDC4221DCC2A}" name="Sprint" dataDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{D6670E8A-4039-4A31-A647-3D365CB5F2AA}" name="Status" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{28AF7159-0180-4285-9018-923AACB2F75B}" name="Responsável" dataDxfId="14"/>
-    <tableColumn id="6" xr3:uid="{FB961424-78DB-4B77-AA3E-E371EBCFF2CC}" name="Matéria" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{04F91C54-26E1-4063-B34C-03486B3A493F}" name="Tamanho (#)" dataDxfId="25"/>
+    <tableColumn id="8" xr3:uid="{203EEE87-31C9-4EC2-8FF5-1485A10738C6}" name="Prioridade" dataDxfId="24"/>
+    <tableColumn id="10" xr3:uid="{BD2690E1-9135-40F1-9CE5-CDC4221DCC2A}" name="Sprint" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{D6670E8A-4039-4A31-A647-3D365CB5F2AA}" name="Status" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{28AF7159-0180-4285-9018-923AACB2F75B}" name="Responsável" dataDxfId="21"/>
+    <tableColumn id="6" xr3:uid="{FB961424-78DB-4B77-AA3E-E371EBCFF2CC}" name="Matéria" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{180FB5DC-F8E5-4FC4-BB23-2BF960AE638A}" name="Tabela1" displayName="Tabela1" ref="B4:D7" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11" tableBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{180FB5DC-F8E5-4FC4-BB23-2BF960AE638A}" name="Tabela1" displayName="Tabela1" ref="B4:D7" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18" tableBorderDxfId="16">
   <autoFilter ref="B4:D7" xr:uid="{180FB5DC-F8E5-4FC4-BB23-2BF960AE638A}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{0D57DA25-020F-4C9B-A627-0D833E1EF48E}" name="Sprint" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{012F0C2B-9F15-43EB-8733-D8818A69C29D}" name="Pontos Planejados" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{8F37F712-2BBC-4C58-ABF5-9A8326EB5006}" name="Pontos Realizados" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{0D57DA25-020F-4C9B-A627-0D833E1EF48E}" name="Sprint" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{012F0C2B-9F15-43EB-8733-D8818A69C29D}" name="Pontos Planejados" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{8F37F712-2BBC-4C58-ABF5-9A8326EB5006}" name="Pontos Realizados" dataDxfId="13"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{309E2AE7-2DA6-4B79-8994-7D1D66D6508B}" name="Tabela14" displayName="Tabela14" ref="B4:D8" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11" headerRowBorderDxfId="9" tableBorderDxfId="10">
+  <autoFilter ref="B4:D8" xr:uid="{180FB5DC-F8E5-4FC4-BB23-2BF960AE638A}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{69477932-3E4B-499A-B551-09FF891D1AE2}" name="Sprint" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{DB1DEAE6-A48D-408F-B8EC-8ED732A4AF2A}" name="Pontos Planejados" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{61D8B7C1-D85B-4290-8F34-BF5A6336A40F}" name="Pontos Realizados" dataDxfId="6">
+      <calculatedColumnFormula>SUMIF(Backlog!$G:$G,B5,Backlog!$E:$E)</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2781,26 +4380,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M51"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="58.453125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="58.44140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="48" style="1" customWidth="1"/>
-    <col min="3" max="7" width="19.81640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="17.453125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="25.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="19.77734375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="17.44140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="25.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="31" style="1" customWidth="1"/>
-    <col min="11" max="11" width="8.81640625" style="1"/>
-    <col min="12" max="12" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="8.81640625" style="1"/>
+    <col min="11" max="11" width="8.77734375" style="1"/>
+    <col min="12" max="12" width="11.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
         <v>17</v>
       </c>
@@ -2814,7 +4413,7 @@
       <c r="I1" s="18"/>
       <c r="J1" s="18"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>61</v>
       </c>
@@ -2846,7 +4445,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="31" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -2879,7 +4478,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" ht="45" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
@@ -2912,7 +4511,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" ht="45" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
@@ -2945,7 +4544,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="62" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" ht="60" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
@@ -2978,7 +4577,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" ht="45" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
@@ -3012,7 +4611,7 @@
       </c>
       <c r="L7" s="5"/>
     </row>
-    <row r="8" spans="1:13" ht="31" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
@@ -3045,7 +4644,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" ht="45" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>0</v>
       </c>
@@ -3079,7 +4678,7 @@
       </c>
       <c r="M9"/>
     </row>
-    <row r="10" spans="1:13" ht="31" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>13</v>
       </c>
@@ -3112,7 +4711,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" ht="45" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>8</v>
       </c>
@@ -3145,7 +4744,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="31" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" ht="30" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>4</v>
       </c>
@@ -3178,7 +4777,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="31" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" ht="30" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>11</v>
       </c>
@@ -3211,7 +4810,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="31" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" ht="30" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>12</v>
       </c>
@@ -3244,7 +4843,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="31" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>54</v>
       </c>
@@ -3277,7 +4876,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" ht="45" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>53</v>
       </c>
@@ -3310,7 +4909,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="31" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>22</v>
       </c>
@@ -3343,7 +4942,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" ht="45" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>23</v>
       </c>
@@ -3376,7 +4975,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" ht="45" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>56</v>
       </c>
@@ -3409,7 +5008,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="31" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>26</v>
       </c>
@@ -3442,7 +5041,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" ht="45" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>27</v>
       </c>
@@ -3475,7 +5074,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>18</v>
       </c>
@@ -3508,7 +5107,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" ht="45" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>19</v>
       </c>
@@ -3541,7 +5140,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="31" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" ht="30" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>42</v>
       </c>
@@ -3574,7 +5173,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="31" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" ht="30" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>25</v>
       </c>
@@ -3607,7 +5206,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="31" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" ht="30" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>57</v>
       </c>
@@ -3640,7 +5239,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>28</v>
       </c>
@@ -3673,7 +5272,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="31" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" ht="30" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>29</v>
       </c>
@@ -3706,7 +5305,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="31" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" ht="30" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>24</v>
       </c>
@@ -3739,7 +5338,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>30</v>
       </c>
@@ -3772,7 +5371,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
         <v>20</v>
       </c>
@@ -3805,7 +5404,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="31" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" ht="30" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
         <v>21</v>
       </c>
@@ -3838,7 +5437,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="31" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" ht="30" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
         <v>2</v>
       </c>
@@ -3871,7 +5470,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
         <v>47</v>
       </c>
@@ -3904,7 +5503,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
         <v>46</v>
       </c>
@@ -3937,7 +5536,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
         <v>45</v>
       </c>
@@ -3970,7 +5569,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
         <v>43</v>
       </c>
@@ -4003,7 +5602,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
         <v>48</v>
       </c>
@@ -4036,7 +5635,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
         <v>49</v>
       </c>
@@ -4069,7 +5668,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
         <v>50</v>
       </c>
@@ -4102,7 +5701,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
         <v>51</v>
       </c>
@@ -4135,7 +5734,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
         <v>44</v>
       </c>
@@ -4168,7 +5767,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="31" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" ht="30" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
         <v>62</v>
       </c>
@@ -4201,7 +5800,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
         <v>94</v>
       </c>
@@ -4234,7 +5833,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
         <v>95</v>
       </c>
@@ -4267,7 +5866,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
         <v>19</v>
       </c>
@@ -4300,7 +5899,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
         <v>96</v>
       </c>
@@ -4333,7 +5932,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
         <v>97</v>
       </c>
@@ -4366,7 +5965,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
         <v>98</v>
       </c>
@@ -4399,7 +5998,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
         <v>99</v>
       </c>
@@ -4432,7 +6031,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="s">
         <v>100</v>
       </c>
@@ -4527,20 +6126,20 @@
   <dimension ref="B2:D9"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.453125" style="9" customWidth="1"/>
-    <col min="2" max="2" width="9.54296875" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.81640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.26953125" style="9" customWidth="1"/>
-    <col min="5" max="16384" width="8.7265625" style="9"/>
+    <col min="1" max="1" width="4.44140625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.77734375" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.21875" style="9" customWidth="1"/>
+    <col min="5" max="16384" width="8.77734375" style="9"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B3" s="10" t="s">
         <v>113</v>
       </c>
@@ -4553,7 +6152,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="4" spans="2:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="13" t="s">
         <v>16</v>
       </c>
@@ -4564,7 +6163,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="9">
         <v>1</v>
       </c>
@@ -4576,7 +6175,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="9">
         <v>2</v>
       </c>
@@ -4588,7 +6187,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="9">
         <v>3</v>
       </c>
@@ -4600,14 +6199,119 @@
         <v>133</v>
       </c>
     </row>
-    <row r="8" spans="2:4" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="9" spans="2:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="10" t="s">
         <v>110</v>
       </c>
       <c r="C9" s="16">
         <f>D3/3</f>
         <v>117.33333333333333</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D5885AC-65BF-4FEC-948C-1DF1DD81DD68}">
+  <dimension ref="B2:D10"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="R17" sqref="R17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.44140625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.77734375" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.21875" style="9" customWidth="1"/>
+    <col min="5" max="16384" width="8.77734375" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B3" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="C3" s="11">
+        <f>SUM(C5:C8)</f>
+        <v>116</v>
+      </c>
+      <c r="D3" s="12">
+        <f>SUM(D5:D8)</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="C5" s="9">
+        <v>29</v>
+      </c>
+      <c r="D5" s="9">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="C6" s="9">
+        <v>29</v>
+      </c>
+      <c r="D6" s="9">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="C7" s="9">
+        <v>29</v>
+      </c>
+      <c r="D7" s="9">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="C8" s="9">
+        <v>29</v>
+      </c>
+      <c r="D8" s="9">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="C10" s="16">
+        <f>117/4</f>
+        <v>29.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualizando a situação dos requisitos no backlog
</commit_message>
<xml_diff>
--- a/Documentação/Backlog/Backlog - Grupo 04.xlsx
+++ b/Documentação/Backlog/Backlog - Grupo 04.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpfer\OneDrive\Documentos\SPTECH\PI\SPRINT\Sprint-SPTECH\Documentação\Backlog\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Desktop\Git\Meus-repositorios\Projeto_PI\sprint2 e sprint3\Documentação\Backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE2EAAA9-2B34-42D8-805E-B46A6C434DB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA25DD18-CA8D-425C-BC09-2B7A5BF42450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="760" yWindow="760" windowWidth="14400" windowHeight="7270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
     <sheet name="Burndow" sheetId="2" r:id="rId2"/>
-    <sheet name="Burndow - Sprint2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -60,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="114">
   <si>
     <t>Configuração e instalação do Arduino Uno R3 com Sensor MQ-2 utilizando Protoboard e 3 Jumpers (Macho-Macho).</t>
   </si>
@@ -402,25 +401,13 @@
   </si>
   <si>
     <t>TOTAL</t>
-  </si>
-  <si>
-    <t>2A</t>
-  </si>
-  <si>
-    <t>2B</t>
-  </si>
-  <si>
-    <t>2C</t>
-  </si>
-  <si>
-    <t>2D</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -463,6 +450,12 @@
       <b/>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -598,7 +591,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -654,11 +647,14 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="32">
+  <dxfs count="25">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -718,122 +714,6 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="medium">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="medium">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="medium">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="medium">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFCB0000"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -2010,863 +1890,6 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="pt-BR"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1260" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="pt-BR" b="1"/>
-              <a:t>BURNDOW</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="3.5833333333333117E-3"/>
-          <c:y val="1.3888888888888888E-2"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1260" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="pt-BR"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="7.0914260717410318E-2"/>
-          <c:y val="0.24520888013998252"/>
-          <c:w val="0.89019685039370078"/>
-          <c:h val="0.67053988043161272"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Burndow - Sprint2'!$B$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>TOTAL</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="bg1">
-                  <a:lumMod val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dLbls>
-            <c:delete val="1"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>'Burndow - Sprint2'!$B$3:$B$8</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>('Burndow - Sprint2'!$B$3,'Burndow - Sprint2'!$B$5:$B$8)</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>TOTAL</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2A</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2B</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2C</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2D</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>'Burndow - Sprint2'!$B$3:$B$8</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>('Burndow - Sprint2'!$B$3,'Burndow - Sprint2'!$B$5:$B$8)</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-22E1-4CBE-B438-D71EBB8520F0}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Burndow - Sprint2'!$C$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Pontos Planejados</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dLbls>
-            <c:dLbl>
-              <c:idx val="0"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-4.8166666666666691E-2"/>
-                  <c:y val="-5.7835739282589678E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000001-22E1-4CBE-B438-D71EBB8520F0}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="2"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-4.2611111111111113E-2"/>
-                  <c:y val="3.01272236803732E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000002-22E1-4CBE-B438-D71EBB8520F0}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="3"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-5.0944444444444445E-2"/>
-                  <c:y val="2.5497594050743571E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000003-22E1-4CBE-B438-D71EBB8520F0}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="4"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-2.7500235563576936E-2"/>
-                  <c:y val="-9.5375773277822738E-3"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{0000000B-22E1-4CBE-B438-D71EBB8520F0}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:sysClr val="windowText" lastClr="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="pt-BR"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="t"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>'Burndow - Sprint2'!$B$3:$B$8</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>('Burndow - Sprint2'!$B$3,'Burndow - Sprint2'!$B$5:$B$8)</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>TOTAL</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2A</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2B</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2C</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2D</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>'Burndow - Sprint2'!$C$3:$C$8</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>('Burndow - Sprint2'!$C$3,'Burndow - Sprint2'!$C$5:$C$8)</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>116</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>29</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-22E1-4CBE-B438-D71EBB8520F0}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Burndow - Sprint2'!$D$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Pontos Realizados</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:srgbClr val="0070C0"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dLbls>
-            <c:dLbl>
-              <c:idx val="0"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-5.0944444444444445E-2"/>
-                  <c:y val="3.9386482939632504E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000005-22E1-4CBE-B438-D71EBB8520F0}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="1"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-3.3500000000000002E-2"/>
-                  <c:y val="3.4756853310002833E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000006-22E1-4CBE-B438-D71EBB8520F0}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="2"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-4.5388888888888888E-2"/>
-                  <c:y val="-3.0057961504811985E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000007-22E1-4CBE-B438-D71EBB8520F0}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="3"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-4.2611111111111113E-2"/>
-                  <c:y val="-3.4687591134441531E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000008-22E1-4CBE-B438-D71EBB8520F0}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="4"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-2.7500235563576936E-2"/>
-                  <c:y val="-6.9196883870551534E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{0000000A-22E1-4CBE-B438-D71EBB8520F0}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:sysClr val="windowText" lastClr="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="pt-BR"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="t"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="0"/>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>'Burndow - Sprint2'!$B$3:$B$8</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>('Burndow - Sprint2'!$B$3,'Burndow - Sprint2'!$B$5:$B$8)</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>TOTAL</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2A</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2B</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2C</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2D</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>'Burndow - Sprint2'!$D$3:$D$8</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>('Burndow - Sprint2'!$D$3,'Burndow - Sprint2'!$D$5:$D$8)</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>35</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000009-22E1-4CBE-B438-D71EBB8520F0}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:dLblPos val="t"/>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="1"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="1937044160"/>
-        <c:axId val="1937044640"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="1937044160"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="pt-BR"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1937044640"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="1937044640"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="pt-BR"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1937044160"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.67850743657042856"/>
-          <c:y val="2.3726305045202681E-2"/>
-          <c:w val="0.32076268591426071"/>
-          <c:h val="0.25868110236220471"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="pt-BR"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:srgbClr val="CB0000"/>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr sz="1050">
-          <a:solidFill>
-            <a:sysClr val="windowText" lastClr="000000"/>
-          </a:solidFill>
-          <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-          <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-        </a:defRPr>
-      </a:pPr>
-      <a:endParaRPr lang="pt-BR"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2907,563 +1930,7 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4020,51 +2487,8 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>250824</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>1586</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>251460</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>7619</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Gráfico 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A26A1CD-D56A-404D-AF02-F3009ABDC1FC}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6A7E6C11-E15E-43D4-8193-0A9DA9700B3C}" name="Tabela2" displayName="Tabela2" ref="A2:J51" totalsRowShown="0" headerRowDxfId="31" tableBorderDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6A7E6C11-E15E-43D4-8193-0A9DA9700B3C}" name="Tabela2" displayName="Tabela2" ref="A2:J51" totalsRowShown="0" headerRowDxfId="24" tableBorderDxfId="23">
   <autoFilter ref="A2:J51" xr:uid="{6A7E6C11-E15E-43D4-8193-0A9DA9700B3C}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:J43">
     <sortCondition ref="G3:G43"/>
@@ -4072,44 +2496,30 @@
     <sortCondition ref="F3:F43"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{9F7D184E-A2F2-4E3C-AF8D-4C0F7A1EB03C}" name="Requisito" dataDxfId="29"/>
-    <tableColumn id="9" xr3:uid="{B9B864BA-C5E5-45E2-817E-3E3871CAC849}" name="Descrição" dataDxfId="28"/>
-    <tableColumn id="2" xr3:uid="{7736CB43-35DE-44E3-99F9-A059BE9A77F6}" name="Classificação" dataDxfId="27"/>
-    <tableColumn id="7" xr3:uid="{3502BB37-E611-4076-B136-7B67D26992FF}" name="Tamanho " dataDxfId="26">
+    <tableColumn id="1" xr3:uid="{9F7D184E-A2F2-4E3C-AF8D-4C0F7A1EB03C}" name="Requisito" dataDxfId="22"/>
+    <tableColumn id="9" xr3:uid="{B9B864BA-C5E5-45E2-817E-3E3871CAC849}" name="Descrição" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{7736CB43-35DE-44E3-99F9-A059BE9A77F6}" name="Classificação" dataDxfId="20"/>
+    <tableColumn id="7" xr3:uid="{3502BB37-E611-4076-B136-7B67D26992FF}" name="Tamanho " dataDxfId="19">
       <calculatedColumnFormula array="1">_xlfn.IFS(E3=3,"PP",E3=5,"P",E3=8,"M",E3=13,"G",E3=21,"GG")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{04F91C54-26E1-4063-B34C-03486B3A493F}" name="Tamanho (#)" dataDxfId="25"/>
-    <tableColumn id="8" xr3:uid="{203EEE87-31C9-4EC2-8FF5-1485A10738C6}" name="Prioridade" dataDxfId="24"/>
-    <tableColumn id="10" xr3:uid="{BD2690E1-9135-40F1-9CE5-CDC4221DCC2A}" name="Sprint" dataDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{D6670E8A-4039-4A31-A647-3D365CB5F2AA}" name="Status" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{28AF7159-0180-4285-9018-923AACB2F75B}" name="Responsável" dataDxfId="21"/>
-    <tableColumn id="6" xr3:uid="{FB961424-78DB-4B77-AA3E-E371EBCFF2CC}" name="Matéria" dataDxfId="20"/>
+    <tableColumn id="5" xr3:uid="{04F91C54-26E1-4063-B34C-03486B3A493F}" name="Tamanho (#)" dataDxfId="18"/>
+    <tableColumn id="8" xr3:uid="{203EEE87-31C9-4EC2-8FF5-1485A10738C6}" name="Prioridade" dataDxfId="17"/>
+    <tableColumn id="10" xr3:uid="{BD2690E1-9135-40F1-9CE5-CDC4221DCC2A}" name="Sprint" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{D6670E8A-4039-4A31-A647-3D365CB5F2AA}" name="Status" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{28AF7159-0180-4285-9018-923AACB2F75B}" name="Responsável" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{FB961424-78DB-4B77-AA3E-E371EBCFF2CC}" name="Matéria" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{180FB5DC-F8E5-4FC4-BB23-2BF960AE638A}" name="Tabela1" displayName="Tabela1" ref="B4:D7" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18" tableBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{180FB5DC-F8E5-4FC4-BB23-2BF960AE638A}" name="Tabela1" displayName="Tabela1" ref="B4:D7" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11" tableBorderDxfId="9">
   <autoFilter ref="B4:D7" xr:uid="{180FB5DC-F8E5-4FC4-BB23-2BF960AE638A}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{0D57DA25-020F-4C9B-A627-0D833E1EF48E}" name="Sprint" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{012F0C2B-9F15-43EB-8733-D8818A69C29D}" name="Pontos Planejados" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{8F37F712-2BBC-4C58-ABF5-9A8326EB5006}" name="Pontos Realizados" dataDxfId="13"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{309E2AE7-2DA6-4B79-8994-7D1D66D6508B}" name="Tabela14" displayName="Tabela14" ref="B4:D8" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11" headerRowBorderDxfId="9" tableBorderDxfId="10">
-  <autoFilter ref="B4:D8" xr:uid="{180FB5DC-F8E5-4FC4-BB23-2BF960AE638A}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{69477932-3E4B-499A-B551-09FF891D1AE2}" name="Sprint" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{DB1DEAE6-A48D-408F-B8EC-8ED732A4AF2A}" name="Pontos Planejados" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{61D8B7C1-D85B-4290-8F34-BF5A6336A40F}" name="Pontos Realizados" dataDxfId="6">
-      <calculatedColumnFormula>SUMIF(Backlog!$G:$G,B5,Backlog!$E:$E)</calculatedColumnFormula>
-    </tableColumn>
+    <tableColumn id="1" xr3:uid="{0D57DA25-020F-4C9B-A627-0D833E1EF48E}" name="Sprint" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{012F0C2B-9F15-43EB-8733-D8818A69C29D}" name="Pontos Planejados" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{8F37F712-2BBC-4C58-ABF5-9A8326EB5006}" name="Pontos Realizados" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4380,26 +2790,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M51"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A35" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H51" sqref="H51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="58.44140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="58.453125" style="1" customWidth="1"/>
     <col min="2" max="2" width="48" style="1" customWidth="1"/>
-    <col min="3" max="7" width="19.77734375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="17.44140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="25.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="19.81640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="17.453125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="25.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="31" style="1" customWidth="1"/>
-    <col min="11" max="11" width="8.77734375" style="1"/>
-    <col min="12" max="12" width="11.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="8.77734375" style="1"/>
+    <col min="11" max="11" width="8.81640625" style="1"/>
+    <col min="12" max="12" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="17" t="s">
         <v>17</v>
       </c>
@@ -4413,7 +2823,7 @@
       <c r="I1" s="18"/>
       <c r="J1" s="18"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>61</v>
       </c>
@@ -4445,7 +2855,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -4478,7 +2888,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
@@ -4511,7 +2921,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
@@ -4544,7 +2954,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="60" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="62" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
@@ -4577,7 +2987,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
@@ -4611,7 +3021,7 @@
       </c>
       <c r="L7" s="5"/>
     </row>
-    <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
@@ -4644,7 +3054,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>0</v>
       </c>
@@ -4678,7 +3088,7 @@
       </c>
       <c r="M9"/>
     </row>
-    <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>13</v>
       </c>
@@ -4711,7 +3121,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>8</v>
       </c>
@@ -4744,7 +3154,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="30" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>4</v>
       </c>
@@ -4777,7 +3187,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="30" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>11</v>
       </c>
@@ -4810,7 +3220,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="30" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>12</v>
       </c>
@@ -4843,7 +3253,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>54</v>
       </c>
@@ -4867,7 +3277,7 @@
         <v>2</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I15" s="2" t="s">
         <v>103</v>
@@ -4876,7 +3286,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>53</v>
       </c>
@@ -4909,7 +3319,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" ht="31" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>22</v>
       </c>
@@ -4933,7 +3343,7 @@
         <v>2</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I17" s="2" t="s">
         <v>106</v>
@@ -4942,7 +3352,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="45" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>23</v>
       </c>
@@ -4966,7 +3376,7 @@
         <v>2</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I18" s="2" t="s">
         <v>104</v>
@@ -4975,7 +3385,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="45" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
         <v>56</v>
       </c>
@@ -5008,7 +3418,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" ht="31" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
         <v>26</v>
       </c>
@@ -5041,7 +3451,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="45" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
         <v>27</v>
       </c>
@@ -5074,7 +3484,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
         <v>18</v>
       </c>
@@ -5107,7 +3517,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="45" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
         <v>19</v>
       </c>
@@ -5131,7 +3541,7 @@
         <v>2</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I23" s="2" t="s">
         <v>104</v>
@@ -5140,7 +3550,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="30" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" ht="31" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
         <v>42</v>
       </c>
@@ -5173,7 +3583,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="30" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" ht="31" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
         <v>25</v>
       </c>
@@ -5206,7 +3616,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="30" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" ht="31" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
         <v>57</v>
       </c>
@@ -5239,7 +3649,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="s">
         <v>28</v>
       </c>
@@ -5272,7 +3682,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="30" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" ht="31" x14ac:dyDescent="0.35">
       <c r="A28" s="4" t="s">
         <v>29</v>
       </c>
@@ -5305,7 +3715,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="30" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" ht="31" x14ac:dyDescent="0.35">
       <c r="A29" s="4" t="s">
         <v>24</v>
       </c>
@@ -5329,7 +3739,7 @@
         <v>2</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I29" s="2" t="s">
         <v>104</v>
@@ -5338,7 +3748,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
         <v>30</v>
       </c>
@@ -5362,7 +3772,7 @@
         <v>2</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I30" s="2" t="s">
         <v>106</v>
@@ -5371,7 +3781,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
         <v>20</v>
       </c>
@@ -5404,7 +3814,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="30" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" ht="31" x14ac:dyDescent="0.35">
       <c r="A32" s="4" t="s">
         <v>21</v>
       </c>
@@ -5437,7 +3847,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="30" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" ht="31" x14ac:dyDescent="0.35">
       <c r="A33" s="4" t="s">
         <v>2</v>
       </c>
@@ -5470,7 +3880,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" s="4" t="s">
         <v>47</v>
       </c>
@@ -5494,7 +3904,7 @@
         <v>3</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I34" s="2" t="s">
         <v>107</v>
@@ -5503,7 +3913,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
         <v>46</v>
       </c>
@@ -5527,7 +3937,7 @@
         <v>3</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I35" s="2" t="s">
         <v>102</v>
@@ -5536,7 +3946,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36" s="4" t="s">
         <v>45</v>
       </c>
@@ -5569,7 +3979,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37" s="4" t="s">
         <v>43</v>
       </c>
@@ -5602,7 +4012,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38" s="4" t="s">
         <v>48</v>
       </c>
@@ -5635,7 +4045,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39" s="4" t="s">
         <v>49</v>
       </c>
@@ -5668,7 +4078,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40" s="4" t="s">
         <v>50</v>
       </c>
@@ -5701,7 +4111,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41" s="4" t="s">
         <v>51</v>
       </c>
@@ -5734,7 +4144,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42" s="4" t="s">
         <v>44</v>
       </c>
@@ -5758,7 +4168,7 @@
         <v>3</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I42" s="2" t="s">
         <v>105</v>
@@ -5767,7 +4177,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="30" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" ht="31" x14ac:dyDescent="0.35">
       <c r="A43" s="4" t="s">
         <v>62</v>
       </c>
@@ -5800,7 +4210,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44" s="4" t="s">
         <v>94</v>
       </c>
@@ -5824,7 +4234,7 @@
         <v>3</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I44" s="2" t="s">
         <v>104</v>
@@ -5833,7 +4243,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A45" s="4" t="s">
         <v>95</v>
       </c>
@@ -5866,7 +4276,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46" s="4" t="s">
         <v>19</v>
       </c>
@@ -5899,7 +4309,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47" s="4" t="s">
         <v>96</v>
       </c>
@@ -5932,7 +4342,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A48" s="4" t="s">
         <v>97</v>
       </c>
@@ -5965,7 +4375,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A49" s="4" t="s">
         <v>98</v>
       </c>
@@ -5998,7 +4408,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A50" s="4" t="s">
         <v>99</v>
       </c>
@@ -6022,7 +4432,7 @@
         <v>3</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I50" s="2" t="s">
         <v>106</v>
@@ -6031,7 +4441,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A51" s="4" t="s">
         <v>100</v>
       </c>
@@ -6054,7 +4464,7 @@
       <c r="G51" s="5">
         <v>3</v>
       </c>
-      <c r="H51" s="2" t="s">
+      <c r="H51" s="19" t="s">
         <v>33</v>
       </c>
       <c r="I51" s="2" t="s">
@@ -6129,17 +4539,17 @@
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.44140625" style="9" customWidth="1"/>
-    <col min="2" max="2" width="9.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.77734375" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.21875" style="9" customWidth="1"/>
-    <col min="5" max="16384" width="8.77734375" style="9"/>
+    <col min="1" max="1" width="4.453125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="9.54296875" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.81640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.1796875" style="9" customWidth="1"/>
+    <col min="5" max="16384" width="8.81640625" style="9"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:4" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B3" s="10" t="s">
         <v>113</v>
       </c>
@@ -6152,7 +4562,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="4" spans="2:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="13" t="s">
         <v>16</v>
       </c>
@@ -6163,7 +4573,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B5" s="9">
         <v>1</v>
       </c>
@@ -6175,7 +4585,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B6" s="9">
         <v>2</v>
       </c>
@@ -6187,7 +4597,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B7" s="9">
         <v>3</v>
       </c>
@@ -6199,119 +4609,14 @@
         <v>133</v>
       </c>
     </row>
-    <row r="8" spans="2:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:4" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="9" spans="2:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B9" s="10" t="s">
         <v>110</v>
       </c>
       <c r="C9" s="16">
         <f>D3/3</f>
         <v>117.33333333333333</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <drawing r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D5885AC-65BF-4FEC-948C-1DF1DD81DD68}">
-  <dimension ref="B2:D10"/>
-  <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="R17" sqref="R17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="4.44140625" style="9" customWidth="1"/>
-    <col min="2" max="2" width="9.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.77734375" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.21875" style="9" customWidth="1"/>
-    <col min="5" max="16384" width="8.77734375" style="9"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B3" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="C3" s="11">
-        <f>SUM(C5:C8)</f>
-        <v>116</v>
-      </c>
-      <c r="D3" s="12">
-        <f>SUM(D5:D8)</f>
-        <v>128</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="C5" s="9">
-        <v>29</v>
-      </c>
-      <c r="D5" s="9">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="C6" s="9">
-        <v>29</v>
-      </c>
-      <c r="D6" s="9">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="C7" s="9">
-        <v>29</v>
-      </c>
-      <c r="D7" s="9">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="C8" s="9">
-        <v>29</v>
-      </c>
-      <c r="D8" s="9">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" ht="15.6" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="C10" s="16">
-        <f>117/4</f>
-        <v>29.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização do backlog do projeto
</commit_message>
<xml_diff>
--- a/Documentação/Backlog/Backlog - Grupo 04.xlsx
+++ b/Documentação/Backlog/Backlog - Grupo 04.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Desktop\Git\Meus-repositorios\Projeto_PI\sprint2 e sprint3\Documentação\Backlog\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VSCode\SPTECH\GitHub\Sprint-SPTECH\Documentação\Backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA25DD18-CA8D-425C-BC09-2B7A5BF42450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3978800-EEB9-4D54-AC98-148BD37B44AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="760" windowWidth="14400" windowHeight="7270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
@@ -641,13 +641,13 @@
     <xf numFmtId="1" fontId="5" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2790,40 +2790,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M51"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A35" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H51" sqref="H51"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="58.453125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="58.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="48" style="1" customWidth="1"/>
-    <col min="3" max="7" width="19.81640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="17.453125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="25.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="19.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="25.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="31" style="1" customWidth="1"/>
-    <col min="11" max="11" width="8.81640625" style="1"/>
-    <col min="12" max="12" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="8.81640625" style="1"/>
+    <col min="11" max="11" width="8.85546875" style="1"/>
+    <col min="12" max="12" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:13" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>61</v>
       </c>
@@ -2855,7 +2855,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="31" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -2888,7 +2888,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
@@ -2921,7 +2921,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
@@ -2954,7 +2954,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="62" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
@@ -2987,7 +2987,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
@@ -3021,7 +3021,7 @@
       </c>
       <c r="L7" s="5"/>
     </row>
-    <row r="8" spans="1:13" ht="31" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
@@ -3054,7 +3054,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>0</v>
       </c>
@@ -3088,7 +3088,7 @@
       </c>
       <c r="M9"/>
     </row>
-    <row r="10" spans="1:13" ht="31" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>13</v>
       </c>
@@ -3121,7 +3121,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>8</v>
       </c>
@@ -3154,7 +3154,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="31" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>4</v>
       </c>
@@ -3187,7 +3187,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="31" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>11</v>
       </c>
@@ -3220,7 +3220,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="31" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>12</v>
       </c>
@@ -3253,7 +3253,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="31" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>54</v>
       </c>
@@ -3286,7 +3286,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>53</v>
       </c>
@@ -3319,7 +3319,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="31" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>22</v>
       </c>
@@ -3352,7 +3352,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>23</v>
       </c>
@@ -3385,7 +3385,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>56</v>
       </c>
@@ -3418,7 +3418,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="31" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>26</v>
       </c>
@@ -3451,7 +3451,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>27</v>
       </c>
@@ -3484,7 +3484,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>18</v>
       </c>
@@ -3517,7 +3517,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>19</v>
       </c>
@@ -3550,7 +3550,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="31" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>42</v>
       </c>
@@ -3583,7 +3583,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="31" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>25</v>
       </c>
@@ -3616,7 +3616,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="31" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>57</v>
       </c>
@@ -3649,7 +3649,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>28</v>
       </c>
@@ -3682,7 +3682,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="31" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>29</v>
       </c>
@@ -3715,7 +3715,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="31" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>24</v>
       </c>
@@ -3748,7 +3748,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>30</v>
       </c>
@@ -3781,7 +3781,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>20</v>
       </c>
@@ -3814,7 +3814,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="31" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>21</v>
       </c>
@@ -3847,7 +3847,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="31" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>2</v>
       </c>
@@ -3880,7 +3880,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>47</v>
       </c>
@@ -3913,7 +3913,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>46</v>
       </c>
@@ -3937,7 +3937,7 @@
         <v>3</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I35" s="2" t="s">
         <v>102</v>
@@ -3946,7 +3946,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>45</v>
       </c>
@@ -3970,7 +3970,7 @@
         <v>3</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I36" s="2" t="s">
         <v>106</v>
@@ -3979,7 +3979,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>43</v>
       </c>
@@ -4003,7 +4003,7 @@
         <v>3</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I37" s="2" t="s">
         <v>104</v>
@@ -4012,7 +4012,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>48</v>
       </c>
@@ -4036,7 +4036,7 @@
         <v>3</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I38" s="2" t="s">
         <v>105</v>
@@ -4045,7 +4045,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>49</v>
       </c>
@@ -4069,7 +4069,7 @@
         <v>3</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I39" s="2" t="s">
         <v>105</v>
@@ -4078,7 +4078,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>50</v>
       </c>
@@ -4102,7 +4102,7 @@
         <v>3</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I40" s="2" t="s">
         <v>107</v>
@@ -4111,7 +4111,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>51</v>
       </c>
@@ -4135,7 +4135,7 @@
         <v>3</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I41" s="2" t="s">
         <v>103</v>
@@ -4144,7 +4144,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>44</v>
       </c>
@@ -4177,7 +4177,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="31" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>62</v>
       </c>
@@ -4210,7 +4210,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>94</v>
       </c>
@@ -4243,7 +4243,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>95</v>
       </c>
@@ -4276,7 +4276,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>19</v>
       </c>
@@ -4300,7 +4300,7 @@
         <v>3</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I46" s="2" t="s">
         <v>104</v>
@@ -4309,7 +4309,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>96</v>
       </c>
@@ -4342,7 +4342,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>97</v>
       </c>
@@ -4366,7 +4366,7 @@
         <v>3</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I48" s="2" t="s">
         <v>102</v>
@@ -4375,7 +4375,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>98</v>
       </c>
@@ -4399,7 +4399,7 @@
         <v>3</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I49" s="2" t="s">
         <v>107</v>
@@ -4408,7 +4408,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>99</v>
       </c>
@@ -4432,7 +4432,7 @@
         <v>3</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I50" s="2" t="s">
         <v>106</v>
@@ -4441,7 +4441,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>100</v>
       </c>
@@ -4464,8 +4464,8 @@
       <c r="G51" s="5">
         <v>3</v>
       </c>
-      <c r="H51" s="19" t="s">
-        <v>33</v>
+      <c r="H51" s="17" t="s">
+        <v>32</v>
       </c>
       <c r="I51" s="2" t="s">
         <v>107</v>
@@ -4539,17 +4539,17 @@
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.453125" style="9" customWidth="1"/>
-    <col min="2" max="2" width="9.54296875" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.81640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.1796875" style="9" customWidth="1"/>
-    <col min="5" max="16384" width="8.81640625" style="9"/>
+    <col min="1" max="1" width="4.42578125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" style="9" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="9"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="10" t="s">
         <v>113</v>
       </c>
@@ -4562,7 +4562,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="4" spans="2:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="13" t="s">
         <v>16</v>
       </c>
@@ -4573,7 +4573,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B5" s="9">
         <v>1</v>
       </c>
@@ -4585,7 +4585,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B6" s="9">
         <v>2</v>
       </c>
@@ -4597,7 +4597,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B7" s="9">
         <v>3</v>
       </c>
@@ -4609,8 +4609,8 @@
         <v>133</v>
       </c>
     </row>
-    <row r="8" spans="2:4" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="9" spans="2:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="2:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
         <v>110</v>
       </c>

</xml_diff>

<commit_message>
Ajustes no Backlog do Projeto
</commit_message>
<xml_diff>
--- a/Documentação/Backlog/Backlog - Grupo 04.xlsx
+++ b/Documentação/Backlog/Backlog - Grupo 04.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VSCode\SPTECH\GitHub\Sprint-SPTECH\Documentação\Backlog\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Desktop\Git\Meus-repositorios\Projeto_PI\Sprint-SPTECH\Documentação\Backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3978800-EEB9-4D54-AC98-148BD37B44AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A48730A8-7CCC-4027-B5A5-E34093C86B53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="110">
   <si>
     <t>Configuração e instalação do Arduino Uno R3 com Sensor MQ-2 utilizando Protoboard e 3 Jumpers (Macho-Macho).</t>
   </si>
@@ -154,15 +154,9 @@
     <t>Validar a solução técnica</t>
   </si>
   <si>
-    <t>Em Andamento</t>
-  </si>
-  <si>
     <t>Finalizada</t>
   </si>
   <si>
-    <t>Pendente</t>
-  </si>
-  <si>
     <t>Matéria</t>
   </si>
   <si>
@@ -220,9 +214,6 @@
     <t>Desejável</t>
   </si>
   <si>
-    <t>Criptografar as senhas inseridas no Banco de Dados</t>
-  </si>
-  <si>
     <t>Colocar máscaras nos inputs de Login e Cadastro</t>
   </si>
   <si>
@@ -287,9 +278,6 @@
   </si>
   <si>
     <t>Máscarar os inputs para facilitar o Insert dos dados no banco e a utilização do usuário</t>
-  </si>
-  <si>
-    <t>Criptografar as senhas inseridos no cadastro do usuário quando enviadas para o banco de dados</t>
   </si>
   <si>
     <t>Telas de Cadastro e Login em HTML, CSS e JS, mas que ainda não enviarão dados para o banco</t>
@@ -1676,13 +1664,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>352</c:v>
+                  <c:v>349</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>124</c:v>
+                  <c:v>121</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>133</c:v>
@@ -2488,12 +2476,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6A7E6C11-E15E-43D4-8193-0A9DA9700B3C}" name="Tabela2" displayName="Tabela2" ref="A2:J51" totalsRowShown="0" headerRowDxfId="24" tableBorderDxfId="23">
-  <autoFilter ref="A2:J51" xr:uid="{6A7E6C11-E15E-43D4-8193-0A9DA9700B3C}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:J43">
-    <sortCondition ref="G3:G43"/>
-    <sortCondition ref="C3:C43"/>
-    <sortCondition ref="F3:F43"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6A7E6C11-E15E-43D4-8193-0A9DA9700B3C}" name="Tabela2" displayName="Tabela2" ref="A2:J50" totalsRowShown="0" headerRowDxfId="24" tableBorderDxfId="23">
+  <autoFilter ref="A2:J50" xr:uid="{6A7E6C11-E15E-43D4-8193-0A9DA9700B3C}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:J42">
+    <sortCondition ref="G3:G42"/>
+    <sortCondition ref="C3:C42"/>
+    <sortCondition ref="F3:F42"/>
   </sortState>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{9F7D184E-A2F2-4E3C-AF8D-4C0F7A1EB03C}" name="Requisito" dataDxfId="22"/>
@@ -2788,28 +2776,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M51"/>
+  <dimension ref="A1:M50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H43" sqref="H43"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A31" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="58.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="58.453125" style="1" customWidth="1"/>
     <col min="2" max="2" width="48" style="1" customWidth="1"/>
-    <col min="3" max="7" width="19.85546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="17.42578125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="25.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="19.81640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="17.453125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="25.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="31" style="1" customWidth="1"/>
-    <col min="11" max="11" width="8.85546875" style="1"/>
-    <col min="12" max="12" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="8.85546875" style="1"/>
+    <col min="11" max="11" width="8.81640625" style="1"/>
+    <col min="12" max="12" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="18" t="s">
         <v>17</v>
       </c>
@@ -2823,9 +2811,9 @@
       <c r="I1" s="19"/>
       <c r="J1" s="19"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>14</v>
@@ -2834,33 +2822,33 @@
         <v>15</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G2" s="8" t="s">
         <v>16</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>1</v>
@@ -2879,21 +2867,21 @@
         <v>1</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>1</v>
@@ -2912,21 +2900,21 @@
         <v>1</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>1</v>
@@ -2945,21 +2933,21 @@
         <v>1</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="62" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>1</v>
@@ -2978,21 +2966,21 @@
         <v>1</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>1</v>
@@ -3011,22 +2999,22 @@
         <v>1</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="L7" s="5"/>
     </row>
-    <row r="8" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>1</v>
@@ -3045,21 +3033,21 @@
         <v>1</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>1</v>
@@ -3078,22 +3066,22 @@
         <v>1</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="M9"/>
     </row>
-    <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>1</v>
@@ -3112,21 +3100,21 @@
         <v>1</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>1</v>
@@ -3145,21 +3133,21 @@
         <v>1</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>1</v>
@@ -3178,21 +3166,21 @@
         <v>1</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>1</v>
@@ -3211,21 +3199,21 @@
         <v>1</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>1</v>
@@ -3244,24 +3232,24 @@
         <v>1</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D15" s="2" t="str" cm="1">
         <f t="array" ref="D15">_xlfn.IFS(E15=3,"PP",E15=5,"P",E15=8,"M",E15=13,"G",E15=21,"GG")</f>
@@ -3277,64 +3265,64 @@
         <v>2</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
-        <v>53</v>
+        <v>22</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>52</v>
+        <v>1</v>
       </c>
       <c r="D16" s="2" t="str" cm="1">
         <f t="array" ref="D16">_xlfn.IFS(E16=3,"PP",E16=5,"P",E16=8,"M",E16=13,"G",E16=21,"GG")</f>
-        <v>PP</v>
+        <v>G</v>
       </c>
       <c r="E16" s="5">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="F16" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G16" s="1">
         <v>2</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D17" s="2" t="str" cm="1">
         <f t="array" ref="D17">_xlfn.IFS(E17=3,"PP",E17=5,"P",E17=8,"M",E17=13,"G",E17=21,"GG")</f>
-        <v>G</v>
+        <v>M</v>
       </c>
       <c r="E17" s="5">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="F17" s="5">
         <v>1</v>
@@ -3343,31 +3331,31 @@
         <v>2</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D18" s="2" t="str" cm="1">
         <f t="array" ref="D18">_xlfn.IFS(E18=3,"PP",E18=5,"P",E18=8,"M",E18=13,"G",E18=21,"GG")</f>
-        <v>M</v>
+        <v>G</v>
       </c>
       <c r="E18" s="5">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F18" s="5">
         <v>1</v>
@@ -3376,31 +3364,31 @@
         <v>2</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="31" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D19" s="2" t="str" cm="1">
         <f t="array" ref="D19">_xlfn.IFS(E19=3,"PP",E19=5,"P",E19=8,"M",E19=13,"G",E19=21,"GG")</f>
-        <v>G</v>
+        <v>PP</v>
       </c>
       <c r="E19" s="5">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="F19" s="5">
         <v>1</v>
@@ -3409,31 +3397,31 @@
         <v>2</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I19" s="2" t="s">
         <v>103</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D20" s="2" t="str" cm="1">
         <f t="array" ref="D20">_xlfn.IFS(E20=3,"PP",E20=5,"P",E20=8,"M",E20=13,"G",E20=21,"GG")</f>
-        <v>PP</v>
+        <v>P</v>
       </c>
       <c r="E20" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F20" s="5">
         <v>1</v>
@@ -3442,31 +3430,31 @@
         <v>2</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D21" s="2" t="str" cm="1">
         <f t="array" ref="D21">_xlfn.IFS(E21=3,"PP",E21=5,"P",E21=8,"M",E21=13,"G",E21=21,"GG")</f>
-        <v>P</v>
+        <v>PP</v>
       </c>
       <c r="E21" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F21" s="5">
         <v>1</v>
@@ -3475,31 +3463,31 @@
         <v>2</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D22" s="2" t="str" cm="1">
         <f t="array" ref="D22">_xlfn.IFS(E22=3,"PP",E22=5,"P",E22=8,"M",E22=13,"G",E22=21,"GG")</f>
-        <v>PP</v>
+        <v>G</v>
       </c>
       <c r="E22" s="5">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="F22" s="5">
         <v>1</v>
@@ -3508,31 +3496,31 @@
         <v>2</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="31" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D23" s="2" t="str" cm="1">
         <f t="array" ref="D23">_xlfn.IFS(E23=3,"PP",E23=5,"P",E23=8,"M",E23=13,"G",E23=21,"GG")</f>
-        <v>G</v>
+        <v>PP</v>
       </c>
       <c r="E23" s="5">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="F23" s="5">
         <v>1</v>
@@ -3541,31 +3529,31 @@
         <v>2</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="31" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D24" s="2" t="str" cm="1">
         <f t="array" ref="D24">_xlfn.IFS(E24=3,"PP",E24=5,"P",E24=8,"M",E24=13,"G",E24=21,"GG")</f>
-        <v>PP</v>
+        <v>P</v>
       </c>
       <c r="E24" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F24" s="5">
         <v>1</v>
@@ -3574,21 +3562,21 @@
         <v>2</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="31" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
-        <v>25</v>
+        <v>54</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>1</v>
@@ -3601,37 +3589,37 @@
         <v>5</v>
       </c>
       <c r="F25" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G25" s="1">
         <v>2</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
-        <v>57</v>
+        <v>28</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D26" s="2" t="str" cm="1">
         <f t="array" ref="D26">_xlfn.IFS(E26=3,"PP",E26=5,"P",E26=8,"M",E26=13,"G",E26=21,"GG")</f>
-        <v>P</v>
+        <v>PP</v>
       </c>
       <c r="E26" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F26" s="5">
         <v>2</v>
@@ -3640,21 +3628,21 @@
         <v>2</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="31" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>1</v>
@@ -3673,31 +3661,31 @@
         <v>2</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="31" x14ac:dyDescent="0.35">
       <c r="A28" s="4" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D28" s="2" t="str" cm="1">
         <f t="array" ref="D28">_xlfn.IFS(E28=3,"PP",E28=5,"P",E28=8,"M",E28=13,"G",E28=21,"GG")</f>
-        <v>PP</v>
+        <v>M</v>
       </c>
       <c r="E28" s="5">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F28" s="5">
         <v>2</v>
@@ -3706,64 +3694,64 @@
         <v>2</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29" s="4" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D29" s="2" t="str" cm="1">
         <f t="array" ref="D29">_xlfn.IFS(E29=3,"PP",E29=5,"P",E29=8,"M",E29=13,"G",E29=21,"GG")</f>
-        <v>M</v>
+        <v>P</v>
       </c>
       <c r="E29" s="5">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F29" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G29" s="1">
         <v>2</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D30" s="2" t="str" cm="1">
         <f t="array" ref="D30">_xlfn.IFS(E30=3,"PP",E30=5,"P",E30=8,"M",E30=13,"G",E30=21,"GG")</f>
-        <v>P</v>
+        <v>M</v>
       </c>
       <c r="E30" s="5">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F30" s="5">
         <v>3</v>
@@ -3772,31 +3760,31 @@
         <v>2</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="31" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D31" s="2" t="str" cm="1">
         <f t="array" ref="D31">_xlfn.IFS(E31=3,"PP",E31=5,"P",E31=8,"M",E31=13,"G",E31=21,"GG")</f>
-        <v>M</v>
+        <v>P</v>
       </c>
       <c r="E31" s="5">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F31" s="5">
         <v>3</v>
@@ -3805,31 +3793,31 @@
         <v>2</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="31" x14ac:dyDescent="0.35">
       <c r="A32" s="4" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="D32" s="2" t="str" cm="1">
         <f t="array" ref="D32">_xlfn.IFS(E32=3,"PP",E32=5,"P",E32=8,"M",E32=13,"G",E32=21,"GG")</f>
-        <v>P</v>
+        <v>G</v>
       </c>
       <c r="E32" s="5">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="F32" s="5">
         <v>3</v>
@@ -3838,54 +3826,54 @@
         <v>2</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I32" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A33" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B33" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="J32" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>93</v>
-      </c>
       <c r="C33" s="2" t="s">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="D33" s="2" t="str" cm="1">
         <f t="array" ref="D33">_xlfn.IFS(E33=3,"PP",E33=5,"P",E33=8,"M",E33=13,"G",E33=21,"GG")</f>
-        <v>G</v>
+        <v>P</v>
       </c>
       <c r="E33" s="5">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="F33" s="5">
+        <v>1</v>
+      </c>
+      <c r="G33" s="1">
         <v>3</v>
       </c>
-      <c r="G33" s="1">
-        <v>2</v>
-      </c>
       <c r="H33" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I33" s="2" t="s">
         <v>103</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>1</v>
@@ -3904,31 +3892,31 @@
         <v>3</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D35" s="2" t="str" cm="1">
         <f t="array" ref="D35">_xlfn.IFS(E35=3,"PP",E35=5,"P",E35=8,"M",E35=13,"G",E35=21,"GG")</f>
-        <v>P</v>
+        <v>G</v>
       </c>
       <c r="E35" s="5">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="F35" s="5">
         <v>1</v>
@@ -3943,28 +3931,28 @@
         <v>102</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D36" s="2" t="str" cm="1">
         <f t="array" ref="D36">_xlfn.IFS(E36=3,"PP",E36=5,"P",E36=8,"M",E36=13,"G",E36=21,"GG")</f>
-        <v>G</v>
+        <v>M</v>
       </c>
       <c r="E36" s="5">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="F36" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G36" s="1">
         <v>3</v>
@@ -3973,18 +3961,18 @@
         <v>31</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37" s="4" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>1</v>
@@ -3997,27 +3985,27 @@
         <v>8</v>
       </c>
       <c r="F37" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G37" s="1">
         <v>3</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I37" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="J37" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A38" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B38" s="4" t="s">
         <v>104</v>
-      </c>
-      <c r="J37" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>108</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>1</v>
@@ -4039,28 +4027,28 @@
         <v>31</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D39" s="2" t="str" cm="1">
         <f t="array" ref="D39">_xlfn.IFS(E39=3,"PP",E39=5,"P",E39=8,"M",E39=13,"G",E39=21,"GG")</f>
-        <v>M</v>
+        <v>P</v>
       </c>
       <c r="E39" s="5">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F39" s="5">
         <v>3</v>
@@ -4072,28 +4060,28 @@
         <v>31</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D40" s="2" t="str" cm="1">
         <f t="array" ref="D40">_xlfn.IFS(E40=3,"PP",E40=5,"P",E40=8,"M",E40=13,"G",E40=21,"GG")</f>
-        <v>P</v>
+        <v>M</v>
       </c>
       <c r="E40" s="5">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F40" s="5">
         <v>3</v>
@@ -4105,28 +4093,28 @@
         <v>31</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41" s="4" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D41" s="2" t="str" cm="1">
         <f t="array" ref="D41">_xlfn.IFS(E41=3,"PP",E41=5,"P",E41=8,"M",E41=13,"G",E41=21,"GG")</f>
-        <v>M</v>
+        <v>P</v>
       </c>
       <c r="E41" s="5">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F41" s="5">
         <v>3</v>
@@ -4138,163 +4126,163 @@
         <v>31</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J41" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" ht="31" x14ac:dyDescent="0.35">
       <c r="A42" s="4" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="D42" s="2" t="str" cm="1">
         <f t="array" ref="D42">_xlfn.IFS(E42=3,"PP",E42=5,"P",E42=8,"M",E42=13,"G",E42=21,"GG")</f>
-        <v>P</v>
+        <v>G</v>
       </c>
       <c r="E42" s="5">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="F42" s="5">
         <v>3</v>
       </c>
-      <c r="G42" s="1">
+      <c r="G42" s="5">
         <v>3</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43" s="4" t="s">
-        <v>62</v>
+        <v>90</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="D43" s="2" t="str" cm="1">
         <f t="array" ref="D43">_xlfn.IFS(E43=3,"PP",E43=5,"P",E43=8,"M",E43=13,"G",E43=21,"GG")</f>
-        <v>G</v>
+        <v>P</v>
       </c>
       <c r="E43" s="5">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="F43" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G43" s="5">
         <v>3</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J43" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44" s="4" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D44" s="2" t="str" cm="1">
         <f t="array" ref="D44">_xlfn.IFS(E44=3,"PP",E44=5,"P",E44=8,"M",E44=13,"G",E44=21,"GG")</f>
-        <v>P</v>
+        <v>M</v>
       </c>
       <c r="E44" s="5">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F44" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G44" s="5">
         <v>3</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I44" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="J44" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A45" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B45" s="4" t="s">
         <v>104</v>
-      </c>
-      <c r="J44" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>108</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D45" s="2" t="str" cm="1">
         <f t="array" ref="D45">_xlfn.IFS(E45=3,"PP",E45=5,"P",E45=8,"M",E45=13,"G",E45=21,"GG")</f>
-        <v>M</v>
+        <v>G</v>
       </c>
       <c r="E45" s="5">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F45" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G45" s="5">
         <v>3</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46" s="4" t="s">
-        <v>19</v>
+        <v>92</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D46" s="2" t="str" cm="1">
         <f t="array" ref="D46">_xlfn.IFS(E46=3,"PP",E46=5,"P",E46=8,"M",E46=13,"G",E46=21,"GG")</f>
-        <v>G</v>
+        <v>PP</v>
       </c>
       <c r="E46" s="5">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="F46" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G46" s="5">
         <v>3</v>
@@ -4303,64 +4291,64 @@
         <v>31</v>
       </c>
       <c r="I46" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="J46" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A47" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B47" s="4" t="s">
         <v>104</v>
-      </c>
-      <c r="J46" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>108</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D47" s="2" t="str" cm="1">
         <f t="array" ref="D47">_xlfn.IFS(E47=3,"PP",E47=5,"P",E47=8,"M",E47=13,"G",E47=21,"GG")</f>
-        <v>PP</v>
+        <v>P</v>
       </c>
       <c r="E47" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F47" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G47" s="5">
         <v>3</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A48" s="4" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D48" s="2" t="str" cm="1">
         <f t="array" ref="D48">_xlfn.IFS(E48=3,"PP",E48=5,"P",E48=8,"M",E48=13,"G",E48=21,"GG")</f>
-        <v>P</v>
+        <v>M</v>
       </c>
       <c r="E48" s="5">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F48" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G48" s="5">
         <v>3</v>
@@ -4369,61 +4357,61 @@
         <v>31</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A49" s="4" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D49" s="2" t="str" cm="1">
         <f t="array" ref="D49">_xlfn.IFS(E49=3,"PP",E49=5,"P",E49=8,"M",E49=13,"G",E49=21,"GG")</f>
-        <v>M</v>
+        <v>P</v>
       </c>
       <c r="E49" s="5">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F49" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G49" s="5">
         <v>3</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="J49" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A50" s="4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D50" s="2" t="str" cm="1">
         <f t="array" ref="D50">_xlfn.IFS(E50=3,"PP",E50=5,"P",E50=8,"M",E50=13,"G",E50=21,"GG")</f>
-        <v>P</v>
+        <v>M</v>
       </c>
       <c r="E50" s="5">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F50" s="5">
         <v>2</v>
@@ -4431,54 +4419,21 @@
       <c r="G50" s="5">
         <v>3</v>
       </c>
-      <c r="H50" s="2" t="s">
-        <v>32</v>
+      <c r="H50" s="17" t="s">
+        <v>31</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="J50" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D51" s="2" t="str" cm="1">
-        <f t="array" ref="D51">_xlfn.IFS(E51=3,"PP",E51=5,"P",E51=8,"M",E51=13,"G",E51=21,"GG")</f>
-        <v>M</v>
-      </c>
-      <c r="E51" s="5">
-        <v>8</v>
-      </c>
-      <c r="F51" s="5">
-        <v>2</v>
-      </c>
-      <c r="G51" s="5">
-        <v>3</v>
-      </c>
-      <c r="H51" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="I51" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="J51" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:J1"/>
   </mergeCells>
-  <conditionalFormatting sqref="C3:F51 H3:J51">
+  <conditionalFormatting sqref="C3:F50 H3:J50">
     <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>"Essencial"</formula>
     </cfRule>
@@ -4489,7 +4444,7 @@
       <formula>"Importante"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H3:J51">
+  <conditionalFormatting sqref="H3:J50">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Finalizada"</formula>
     </cfRule>
@@ -4501,25 +4456,25 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:G51" xr:uid="{E9CF9112-A7D5-4A3C-8BE7-64942B77F025}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:G50" xr:uid="{E9CF9112-A7D5-4A3C-8BE7-64942B77F025}">
       <formula1>"1,2,3"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C51" xr:uid="{8630AD09-0144-4519-A158-ED3BE3A9872A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C50" xr:uid="{8630AD09-0144-4519-A158-ED3BE3A9872A}">
       <formula1>"Essencial,Importante,Desejável"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H51" xr:uid="{C0662D32-9D3B-4AF6-A8DD-256816F071DB}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H50" xr:uid="{C0662D32-9D3B-4AF6-A8DD-256816F071DB}">
       <formula1>"Pendente,Em Andamento, Finalizada"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J3:J51" xr:uid="{39068AEF-AD2C-49EF-8127-9D7EB96B73B3}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J3:J50" xr:uid="{39068AEF-AD2C-49EF-8127-9D7EB96B73B3}">
       <formula1>"-,Algoritmo,Arquitetura Computacional,Banco de Dados,Introdução à SO,Pesquisa e Inovação,Tecnlogia da Informação"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D51" xr:uid="{14DF18D5-D0D6-460C-9DD3-F79140E2407B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D50" xr:uid="{14DF18D5-D0D6-460C-9DD3-F79140E2407B}">
       <formula1>"PP,P,M,G,GG"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E51" xr:uid="{007AAA73-0A84-4DF3-8313-6B93A73F8B5E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E50" xr:uid="{007AAA73-0A84-4DF3-8313-6B93A73F8B5E}">
       <formula1>"3,5,8,13,21"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I51" xr:uid="{DC5F1E14-E5C2-4B5F-80D3-19B355F02D2D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I50" xr:uid="{DC5F1E14-E5C2-4B5F-80D3-19B355F02D2D}">
       <formula1>"João Pedro, Lucas Aiello, Lucas Pereira, Miguel Angel, Shelly Nadudvari, Thiago Sanchez"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4539,19 +4494,19 @@
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" style="9" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.140625" style="9" customWidth="1"/>
-    <col min="5" max="16384" width="8.85546875" style="9"/>
+    <col min="1" max="1" width="4.453125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="9.54296875" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.81640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.1796875" style="9" customWidth="1"/>
+    <col min="5" max="16384" width="8.81640625" style="9"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B3" s="10" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C3" s="11">
         <f>SUM(C5:C7)</f>
@@ -4559,21 +4514,21 @@
       </c>
       <c r="D3" s="12">
         <f>SUM(D5:D7)</f>
-        <v>352</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="13" t="s">
         <v>16</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B5" s="9">
         <v>1</v>
       </c>
@@ -4585,7 +4540,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B6" s="9">
         <v>2</v>
       </c>
@@ -4594,10 +4549,10 @@
       </c>
       <c r="D6" s="9">
         <f>SUMIF(Backlog!$G:$G,B6,Backlog!$E:$E)</f>
-        <v>124</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B7" s="9">
         <v>3</v>
       </c>
@@ -4609,14 +4564,14 @@
         <v>133</v>
       </c>
     </row>
-    <row r="8" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="2:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:4" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="9" spans="2:4" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B9" s="10" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C9" s="16">
         <f>D3/3</f>
-        <v>117.33333333333333</v>
+        <v>116.33333333333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>